<commit_message>
📊 Update Excel files from OneDrive - 2025-08-27 09:43:07
</commit_message>
<xml_diff>
--- a/data/Daily_Updates.xlsx
+++ b/data/Daily_Updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F79292A-CC9A-469D-94C0-57D868FFAA10}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20CC7C11-0181-4DD2-8CC3-6D77F0523633}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
+    <workbookView minimized="1" xWindow="4800" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Updates" sheetId="1" r:id="rId1"/>
@@ -525,10 +525,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
     <col min="3" max="3" width="29.6328125" customWidth="1"/>
     <col min="4" max="4" width="26.54296875" customWidth="1"/>
     <col min="5" max="5" width="29.6328125" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
     <col min="7" max="7" width="18.26953125" customWidth="1"/>
     <col min="8" max="8" width="18.81640625" customWidth="1"/>
     <col min="9" max="9" width="18.54296875" customWidth="1"/>

</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-08-28 09:42:48
</commit_message>
<xml_diff>
--- a/data/Daily_Updates.xlsx
+++ b/data/Daily_Updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20CC7C11-0181-4DD2-8CC3-6D77F0523633}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47F77AEF-0FB8-4CF9-BFD8-E878843B4001}"/>
   <bookViews>
     <workbookView minimized="1" xWindow="4800" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sections Config" sheetId="2" r:id="rId2"/>
     <sheet name="Team Members" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,9 +55,36 @@
     <t>PRIORITY</t>
   </si>
   <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>ASSIGNED_TO</t>
+  </si>
+  <si>
+    <t>CREATED_BY</t>
+  </si>
+  <si>
+    <t>DUE_DATE</t>
+  </si>
+  <si>
     <t>CERTIFICATIONS</t>
   </si>
   <si>
+    <t>CDF</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>IN PROCESS</t>
+  </si>
+  <si>
+    <t>GK</t>
+  </si>
+  <si>
+    <t>NKC</t>
+  </si>
+  <si>
     <t>NEW PRODUCT DEVELOPMENT</t>
   </si>
   <si>
@@ -79,24 +106,24 @@
     <t>Security</t>
   </si>
   <si>
+    <t>#10b981</t>
+  </si>
+  <si>
     <t>NewReleases</t>
   </si>
   <si>
+    <t>#3b82f6</t>
+  </si>
+  <si>
     <t>School</t>
   </si>
   <si>
+    <t>#f59e0b</t>
+  </si>
+  <si>
     <t>Science</t>
   </si>
   <si>
-    <t>#10b981</t>
-  </si>
-  <si>
-    <t>#3b82f6</t>
-  </si>
-  <si>
-    <t>#f59e0b</t>
-  </si>
-  <si>
     <t>#dc2626</t>
   </si>
   <si>
@@ -104,33 +131,6 @@
   </si>
   <si>
     <t>EMAIL</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>ASSIGNED_TO</t>
-  </si>
-  <si>
-    <t>CREATED_BY</t>
-  </si>
-  <si>
-    <t>CREATED_DATE</t>
-  </si>
-  <si>
-    <t>CDF</t>
-  </si>
-  <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>IN PROCESS</t>
-  </si>
-  <si>
-    <t>GK</t>
-  </si>
-  <si>
-    <t>NKC</t>
   </si>
 </sst>
 </file>
@@ -519,20 +519,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF37F0-237B-49DA-82CE-7792F714DDD8}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="29.6328125" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="29.6328125" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="18.26953125" customWidth="1"/>
-    <col min="8" max="8" width="18.81640625" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -552,16 +552,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -572,22 +572,22 @@
         <v>45896</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="I2" s="1">
         <v>45896</v>
@@ -601,7 +601,7 @@
         <v>45896</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -612,7 +612,7 @@
         <v>45896</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -623,7 +623,7 @@
         <v>45896</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -648,67 +648,67 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="29.81640625" customWidth="1"/>
-    <col min="2" max="2" width="25.90625" customWidth="1"/>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42.95" customHeight="1">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="43" customHeight="1">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="36" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32.1" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="36.6" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="32" customHeight="1">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="36.5" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="40.5" customHeight="1"/>
@@ -725,14 +725,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -744,6 +744,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4CAC9FC675B57408E93BF556641D4D2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274a8390434e2b99e5c0abfa3a3bc86a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32f52b41-3b94-4090-a175-52d6bdf443eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="396c0ffd131d9db66c00cc10498a82b8" ns3:_="">
     <xsd:import namespace="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
@@ -937,15 +946,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -955,43 +955,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75991612-C3F4-41E8-93AA-3DE7B451F1B9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A698D09-50DE-4F71-8AF3-2F1CD67DD4C7}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A698D09-50DE-4F71-8AF3-2F1CD67DD4C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75991612-C3F4-41E8-93AA-3DE7B451F1B9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECBE0542-6209-4F51-9E34-DB4CFCBEE60A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECBE0542-6209-4F51-9E34-DB4CFCBEE60A}"/>
 </file>
</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-01 09:44:54
</commit_message>
<xml_diff>
--- a/data/Daily_Updates.xlsx
+++ b/data/Daily_Updates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{47F77AEF-0FB8-4CF9-BFD8-E878843B4001}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{779C5B63-A43A-47D0-8D77-3B5C238493BE}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4800" yWindow="2810" windowWidth="14400" windowHeight="7270" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Updates" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>CERTIFICATIONS</t>
-  </si>
-  <si>
-    <t>CDF</t>
   </si>
   <si>
     <t>HIGH</t>
@@ -198,6 +195,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -519,20 +520,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF37F0-237B-49DA-82CE-7792F714DDD8}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="29.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" customWidth="1"/>
+    <col min="5" max="5" width="29.54296875" customWidth="1"/>
+    <col min="6" max="6" width="14.7265625" customWidth="1"/>
+    <col min="7" max="7" width="18.26953125" customWidth="1"/>
+    <col min="8" max="8" width="18.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -574,24 +575,19 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1">
-        <v>45896</v>
-      </c>
+      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9">
       <c r="A3">
@@ -601,7 +597,7 @@
         <v>45896</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -612,7 +608,7 @@
         <v>45896</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -623,7 +619,7 @@
         <v>45896</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -648,67 +644,67 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="29.81640625" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" customHeight="1">
       <c r="A1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="42.95" customHeight="1">
+    </row>
+    <row r="2" spans="1:3" ht="43" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="36" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="32.15" customHeight="1">
+      <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="32.1" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="36.65" customHeight="1">
+      <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="36.6" customHeight="1">
-      <c r="A5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="40.5" customHeight="1"/>
@@ -725,14 +721,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -955,13 +951,43 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A698D09-50DE-4F71-8AF3-2F1CD67DD4C7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A698D09-50DE-4F71-8AF3-2F1CD67DD4C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75991612-C3F4-41E8-93AA-3DE7B451F1B9}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75991612-C3F4-41E8-93AA-3DE7B451F1B9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECBE0542-6209-4F51-9E34-DB4CFCBEE60A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECBE0542-6209-4F51-9E34-DB4CFCBEE60A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
📊 Update Excel files from OneDrive - 2025-09-08 09:44:19
</commit_message>
<xml_diff>
--- a/data/Daily_Updates.xlsx
+++ b/data/Daily_Updates.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vikramsolar0-my.sharepoint.com/personal/naveen_chamaria_vikramsolar_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{779C5B63-A43A-47D0-8D77-3B5C238493BE}"/>
+  <xr:revisionPtr revIDLastSave="139" documentId="8_{8601C189-1817-438D-BD84-799E1F3D6A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A182A54-B5EA-423F-8003-7FFE10351F17}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{36554B71-EBEA-4515-9FB7-ABC18DFA4A55}"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Updates" sheetId="1" r:id="rId1"/>
-    <sheet name="Sections Config" sheetId="2" r:id="rId2"/>
-    <sheet name="Team Members" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="Sections Config" sheetId="2" r:id="rId3"/>
+    <sheet name="Team Members" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -128,6 +129,55 @@
   </si>
   <si>
     <t>EMAIL</t>
+  </si>
+  <si>
+    <t>VALLAM</t>
+  </si>
+  <si>
+    <t>FINAL DATE</t>
+  </si>
+  <si>
+    <t>WORK</t>
+  </si>
+  <si>
+    <t>SUPPORT</t>
+  </si>
+  <si>
+    <t>LATEST UPDATE</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT OF QC</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>BD PROCUREMENT</t>
+  </si>
+  <si>
+    <t>NISE/ IIT LETTER</t>
+  </si>
+  <si>
+    <t>IEC and PAN FILE with BD</t>
+  </si>
+  <si>
+    <t>G12R Module being sent from Falta plant and M10R being sent from Chennai Plant
+Modules will be dispatch by 10/09/2025 (Pending SO in Falta custom)</t>
+  </si>
+  <si>
+    <t>MAILED TO QC FOR SENDING THE SAMPLES</t>
+  </si>
+  <si>
+    <t>Atleast by 20/09/2025 - for samples. 15/10/2025 - Large order</t>
+  </si>
+  <si>
+    <t>By today evening we will get the final date</t>
+  </si>
+  <si>
+    <t>Approx 30/11/2025</t>
+  </si>
+  <si>
+    <t>WILL BE COMMUNICATED SOON</t>
   </si>
 </sst>
 </file>
@@ -168,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -179,6 +229,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,7 +573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BF37F0-237B-49DA-82CE-7792F714DDD8}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -637,6 +690,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D062A29-5272-420C-9FC3-1B121FCFE2A2}">
+  <dimension ref="B2:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="20.6328125" customWidth="1"/>
+    <col min="3" max="3" width="27.90625" customWidth="1"/>
+    <col min="4" max="4" width="36.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="58">
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45945</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="58">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE6E8FF8-17BE-4F50-902E-20024914F6D0}">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -713,7 +853,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79DACB9-34D2-495E-8771-874CD6E925DF}">
   <dimension ref="A1:C1"/>
   <sheetViews>
@@ -740,15 +880,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4CAC9FC675B57408E93BF556641D4D2" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="274a8390434e2b99e5c0abfa3a3bc86a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="32f52b41-3b94-4090-a175-52d6bdf443eb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="396c0ffd131d9db66c00cc10498a82b8" ns3:_="">
     <xsd:import namespace="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
@@ -942,6 +1073,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -951,14 +1091,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A698D09-50DE-4F71-8AF3-2F1CD67DD4C7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75991612-C3F4-41E8-93AA-3DE7B451F1B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -976,18 +1108,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A698D09-50DE-4F71-8AF3-2F1CD67DD4C7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECBE0542-6209-4F51-9E34-DB4CFCBEE60A}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="32f52b41-3b94-4090-a175-52d6bdf443eb"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>